<commit_message>
Dodanie okna użytkowników w admin panelu, wyświetlanie wszystkich użytkowników,dodawanie użytkownika
</commit_message>
<xml_diff>
--- a/zabka/Frog/products.xlsx
+++ b/zabka/Frog/products.xlsx
@@ -462,7 +462,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -479,7 +479,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -496,45 +496,53 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>jabkol</t>
+          <t>Czarnuch</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1111</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Robol</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>jabkol</t>
+          <t>da</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1111</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
+        <v>3214</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>dam</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Czarnuch</t>
+          <t xml:space="preserve">czarnuch </t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -545,7 +553,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Robol</t>
+          <t>robol</t>
         </is>
       </c>
     </row>

</xml_diff>